<commit_message>
Correccion dinamico y PL v2
</commit_message>
<xml_diff>
--- a/Input Palas.xlsx
+++ b/Input Palas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Collahuasi-Validador-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF89E38-E24B-44A3-A3F1-D64E5A54ED86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43C4DA0-CAEB-43DE-940F-5467EFA0BEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1175,12 +1175,12 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.54296875" customWidth="1"/>
     <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Dinamico ok PL ok
</commit_message>
<xml_diff>
--- a/Input Palas.xlsx
+++ b/Input Palas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Collahuasi-Validador-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43C4DA0-CAEB-43DE-940F-5467EFA0BEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B9EEEA-E2EA-4DC4-AD55-07E4ADB046AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CS03" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>NP</t>
   </si>
@@ -150,12 +150,6 @@
   </si>
   <si>
     <t>Palomo1</t>
-  </si>
-  <si>
-    <t>Palomo2</t>
-  </si>
-  <si>
-    <t>Palomo3</t>
   </si>
 </sst>
 </file>
@@ -165,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +303,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -655,13 +656,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1172,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1334,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1373,179 +1377,179 @@
         <v>12174</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>303</v>
+      </c>
+      <c r="E5" s="6">
+        <v>9000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>182.04741540000001</v>
+      </c>
+      <c r="G5" s="6">
+        <v>43.517277</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="J5" s="6">
+        <v>2.4423081570997001</v>
+      </c>
+      <c r="K5" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L5" s="6">
+        <v>7.834407158836683</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N5" s="6">
+        <v>3913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>303</v>
+      </c>
+      <c r="E6" s="6">
+        <v>4500</v>
+      </c>
+      <c r="F6" s="6">
+        <v>236.96753819999998</v>
+      </c>
+      <c r="G6" s="6">
+        <v>22.7830206</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1.0471900002617966</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1.8055000004513666</v>
+      </c>
+      <c r="L6" s="6">
+        <v>2.9141403516057331</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N6" s="6">
+        <v>9970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>303</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9000</v>
+      </c>
+      <c r="F7" s="6">
+        <v>233.01076860000001</v>
+      </c>
+      <c r="G7" s="6">
+        <v>16.598233200000003</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.85935322891439003</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1.8055000004513666</v>
+      </c>
+      <c r="L7" s="6">
+        <v>3.0066264617906167</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N7" s="6">
+        <v>9970</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C5">
+      <c r="C8" s="8">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D8" s="8">
         <v>303</v>
       </c>
-      <c r="E5">
+      <c r="E8" s="8">
         <v>9000</v>
       </c>
-      <c r="F5">
-        <v>182.04741540000001</v>
-      </c>
-      <c r="G5">
-        <v>43.517277</v>
-      </c>
-      <c r="H5">
-        <v>0.1</v>
-      </c>
-      <c r="I5">
-        <v>0.12</v>
-      </c>
-      <c r="J5">
-        <v>2.4423081570997001</v>
-      </c>
-      <c r="K5">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="L5">
-        <v>7.834407158836683</v>
-      </c>
-      <c r="M5">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N5">
-        <v>3913</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>303</v>
-      </c>
-      <c r="E6">
-        <v>4500</v>
-      </c>
-      <c r="F6">
-        <v>236.96753819999998</v>
-      </c>
-      <c r="G6">
-        <v>22.7830206</v>
-      </c>
-      <c r="H6">
-        <v>0.08</v>
-      </c>
-      <c r="I6">
-        <v>0.08</v>
-      </c>
-      <c r="J6">
-        <v>1.0471900002617966</v>
-      </c>
-      <c r="K6">
+      <c r="F8" s="8">
+        <v>295.42289099999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>12.1300092</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.86988798963546166</v>
+      </c>
+      <c r="K8" s="8">
         <v>1.8055000004513666</v>
       </c>
-      <c r="L6">
-        <v>2.9141403516057331</v>
-      </c>
-      <c r="M6">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N6">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>303</v>
-      </c>
-      <c r="E7">
-        <v>9000</v>
-      </c>
-      <c r="F7">
-        <v>233.01076860000001</v>
-      </c>
-      <c r="G7">
-        <v>16.598233200000003</v>
-      </c>
-      <c r="H7">
-        <v>0.08</v>
-      </c>
-      <c r="I7">
-        <v>0.1</v>
-      </c>
-      <c r="J7">
-        <v>0.85935322891439003</v>
-      </c>
-      <c r="K7">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="L7">
-        <v>3.0066264617906167</v>
-      </c>
-      <c r="M7">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N7">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>303</v>
-      </c>
-      <c r="E8">
-        <v>9000</v>
-      </c>
-      <c r="F8">
-        <v>295.42289099999999</v>
-      </c>
-      <c r="G8">
-        <v>12.1300092</v>
-      </c>
-      <c r="H8">
-        <v>0.02</v>
-      </c>
-      <c r="I8">
-        <v>0.02</v>
-      </c>
-      <c r="J8">
-        <v>0.86988798963546166</v>
-      </c>
-      <c r="K8">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="L8">
+      <c r="L8" s="8">
         <v>2.9956139320466169</v>
       </c>
-      <c r="M8">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N8">
+      <c r="M8" s="8">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N8" s="8">
         <v>9970</v>
       </c>
     </row>
@@ -1554,12 +1558,12 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>303</v>
       </c>
       <c r="E9" s="5">
@@ -1603,7 +1607,7 @@
       <c r="C10" s="5">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>303</v>
       </c>
       <c r="E10" s="5">
@@ -1637,141 +1641,54 @@
         <v>9970</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="5">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>303</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>9000</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>233.01076860000001</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>16.598233200000003</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>0.08</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>0.1</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="5">
         <v>0.85935322891439003</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>1.8055000004513666</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="5">
         <v>3.0066264617906167</v>
       </c>
-      <c r="M11">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N11">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>303</v>
-      </c>
-      <c r="E12">
-        <v>9000</v>
-      </c>
-      <c r="F12">
-        <v>295.42289099999999</v>
-      </c>
-      <c r="G12">
-        <v>12.1300092</v>
-      </c>
-      <c r="H12">
-        <v>0.02</v>
-      </c>
-      <c r="I12">
-        <v>0.02</v>
-      </c>
-      <c r="J12">
-        <v>0.86988798963546166</v>
-      </c>
-      <c r="K12">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="L12">
-        <v>2.9956139320466169</v>
-      </c>
-      <c r="M12">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N12">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>303</v>
-      </c>
-      <c r="E13" s="5">
-        <v>9000</v>
-      </c>
-      <c r="F13" s="5">
-        <v>250.71384959999997</v>
-      </c>
-      <c r="G13" s="5">
-        <v>18.368355600000001</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0.95447005232195004</v>
-      </c>
-      <c r="K13" s="5">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="L13" s="5">
-        <v>2.9420988937244501</v>
-      </c>
-      <c r="M13" s="5">
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="N13" s="5">
+      <c r="M11" s="5">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N11" s="5">
         <v>9970</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>